<commit_message>
Atualizando o Backlog - Isak de Amorim
</commit_message>
<xml_diff>
--- a/Backlog - PrimeiraSprint.xlsx
+++ b/Backlog - PrimeiraSprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9acbaa33c33b352b/Área de Trabalho/SPTECH/P.I/1º Semestre/BataTech - 1º Semestre/BataTech-Semestre1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{46AE2DA5-FBC9-417D-BA33-8DCEB097D853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3650119B-2CBF-48B1-A23F-23F80FF7CBAA}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{46AE2DA5-FBC9-417D-BA33-8DCEB097D853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71D80FDB-531F-436C-A734-039F9F755D41}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71046EA7-8BF6-4FB3-A79E-EEB4594AAFC2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>Projeto BataTech - Backlog</t>
   </si>
@@ -153,6 +153,90 @@
   </si>
   <si>
     <t>Desejável</t>
+  </si>
+  <si>
+    <t>Instalar MySQL no servidor de dados da solução (VM Linux)</t>
+  </si>
+  <si>
+    <t>Instalar o MySQL no servidor da máquina virtual para inserção dos dados.</t>
+  </si>
+  <si>
+    <t>Inserção de dados do Arduino no MySQL (VM Linux)</t>
+  </si>
+  <si>
+    <t>Inserção dos dados coletados pelos sensores para o banco de dados no servidor.</t>
+  </si>
+  <si>
+    <t>Diagrama da Solução (Validado)</t>
+  </si>
+  <si>
+    <t>Validar o diagrama de solução.</t>
+  </si>
+  <si>
+    <t>Infraestrutura de cliente, servidor utilizando a VM Linux</t>
+  </si>
+  <si>
+    <t>Infraestrutura do cliente funcionando com o servidor utilizando a máquina virtual.</t>
+  </si>
+  <si>
+    <t>Planilha Sprint Backlog</t>
+  </si>
+  <si>
+    <t>Planilha Product Backlog</t>
+  </si>
+  <si>
+    <t>Diagrama da Solução</t>
+  </si>
+  <si>
+    <t>Criar uma planilha com um plano concreto de como atingir a Meta da Sprint, detalhando o trabalho a ser feito e como ele será realizado.</t>
+  </si>
+  <si>
+    <t>Criar uma planilha com uma lista dinâmica e priorizada de todas as necessidades de um produto, como funcionalidades, melhorias e correções.</t>
+  </si>
+  <si>
+    <t>Documento de Mudança</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>Fluxograma do suporte</t>
+  </si>
+  <si>
+    <t>Documento que registra cada mudança solicitada no decorrer do projeto e controla seu status.</t>
+  </si>
+  <si>
+    <t>Criar e automatizar o processo de suporte e atendimento para solucionar problemas e responder a solicitações dos clientes.</t>
+  </si>
+  <si>
+    <t>Criar o fluxograma de como funcionará o suporte ao cliente.</t>
+  </si>
+  <si>
+    <t>Criar um diagrama da solução com os principais elementos da solução, suas interações e como eles contribuem para atender às necessidades de negócio.</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro e Login</t>
+  </si>
+  <si>
+    <t>Tela de Dashboard</t>
+  </si>
+  <si>
+    <t>Criar a tela de cadastro e login do site institucional.</t>
+  </si>
+  <si>
+    <t>Criar Tela de Dashboard dos dados coletados do site institucional.</t>
+  </si>
+  <si>
+    <t>Tabelas criadas no MySQL - Protótipo - Final</t>
+  </si>
+  <si>
+    <t>Protótipo das tabelas de banco de dados definidas para o banco de dados final.</t>
+  </si>
+  <si>
+    <t>Tela de Simulador financeira definida para o site final.</t>
+  </si>
+  <si>
+    <t>Tela de simulador financeiro - Final</t>
   </si>
 </sst>
 </file>
@@ -237,16 +321,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,6 +347,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,211 +670,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3253BF3-9D76-45F5-B21A-7F7BAB520617}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.109375" customWidth="1"/>
-    <col min="2" max="2" width="187.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="194.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>